<commit_message>
renommation d'experimentages dix vert Eva riait
c'est effe titre
</commit_message>
<xml_diff>
--- a/Synthèse-Experiences/ExperimentsMAJ12juillet.xlsx
+++ b/Synthèse-Experiences/ExperimentsMAJ12juillet.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacData/Users/clemencebriosnefrejaville/Desktop/GitHubAustralie/Synthèse-Experiences/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25160" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Resultats" sheetId="1" r:id="rId1"/>
     <sheet name="Interpretations" sheetId="2" r:id="rId2"/>
     <sheet name="Resolution" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF26" authorId="0">
+    <comment ref="AF27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF28" authorId="0">
+    <comment ref="AF31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF32" authorId="0">
+    <comment ref="AF43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -921,7 +916,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1168,12 +1163,6 @@
     <xf numFmtId="0" fontId="6" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1183,6 +1172,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1210,19 +1212,45 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -3530,15 +3558,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:AF60" dataDxfId="79">
-  <autoFilter ref="A3:AF60">
-    <filterColumn colId="3">
-      <filters blank="1">
-        <dateGroupItem year="2016" month="7" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A4:AF33">
-    <sortCondition ref="D3:D33"/>
+  <autoFilter ref="A3:AF60"/>
+  <sortState ref="A4:AF60">
+    <sortCondition ref="A3:A60"/>
   </sortState>
   <tableColumns count="32">
     <tableColumn id="27" name="# Exp" totalsRowLabel="Total" dataDxfId="78" totalsRowDxfId="77"/>
@@ -3937,121 +3959,121 @@
   <dimension ref="A1:AF60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AF48" sqref="AF48"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="6.296875" style="29" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="75" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="69" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="61" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.69921875" style="69" customWidth="1"/>
+    <col min="4" max="4" width="12.69921875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.296875" customWidth="1"/>
+    <col min="9" max="9" width="12.69921875" customWidth="1"/>
+    <col min="10" max="10" width="11.19921875" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="41" customWidth="1"/>
+    <col min="13" max="14" width="10.796875" customWidth="1"/>
+    <col min="15" max="15" width="10.796875" style="41" customWidth="1"/>
     <col min="16" max="16" width="12.5" customWidth="1"/>
-    <col min="17" max="17" width="11.83203125" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.83203125" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" customWidth="1"/>
-    <col min="25" max="25" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.33203125" customWidth="1"/>
-    <col min="29" max="29" width="14.1640625" customWidth="1"/>
-    <col min="30" max="30" width="17.33203125" customWidth="1"/>
-    <col min="31" max="31" width="15.1640625" customWidth="1"/>
-    <col min="32" max="32" width="41.83203125" customWidth="1"/>
+    <col min="17" max="17" width="11.796875" customWidth="1"/>
+    <col min="18" max="18" width="12.796875" customWidth="1"/>
+    <col min="19" max="19" width="11.796875" customWidth="1"/>
+    <col min="20" max="20" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.796875" customWidth="1"/>
+    <col min="22" max="22" width="13.19921875" customWidth="1"/>
+    <col min="23" max="23" width="11.796875" customWidth="1"/>
+    <col min="24" max="24" width="13.19921875" customWidth="1"/>
+    <col min="25" max="25" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.296875" customWidth="1"/>
+    <col min="29" max="29" width="14.19921875" customWidth="1"/>
+    <col min="30" max="30" width="17.296875" customWidth="1"/>
+    <col min="31" max="31" width="15.19921875" customWidth="1"/>
+    <col min="32" max="32" width="41.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="93" t="s">
+      <c r="K1" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="93"/>
+      <c r="L1" s="96"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="37"/>
-      <c r="Q1" s="95" t="s">
+      <c r="Q1" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="96" t="s">
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="97" t="s">
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="97"/>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
       <c r="AD1" s="49" t="s">
         <v>68</v>
       </c>
       <c r="AE1" s="49"/>
     </row>
-    <row r="2" spans="1:32" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H2" s="60"/>
-      <c r="M2" s="98" t="s">
+      <c r="M2" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
       <c r="P2" s="37"/>
-      <c r="Q2" s="99" t="s">
+      <c r="Q2" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99" t="s">
+      <c r="R2" s="102"/>
+      <c r="S2" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="99"/>
-      <c r="U2" s="100" t="s">
+      <c r="T2" s="102"/>
+      <c r="U2" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100" t="s">
+      <c r="V2" s="103"/>
+      <c r="W2" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="101" t="s">
+      <c r="X2" s="103"/>
+      <c r="Y2" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="101"/>
-      <c r="AA2" s="101" t="s">
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="101"/>
-      <c r="AC2" s="94" t="s">
+      <c r="AB2" s="104"/>
+      <c r="AC2" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="AD2" s="94"/>
-      <c r="AE2" s="94"/>
+      <c r="AD2" s="97"/>
+      <c r="AE2" s="97"/>
     </row>
-    <row r="3" spans="1:32" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>77</v>
       </c>
@@ -4149,7 +4171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
         <v>1</v>
       </c>
@@ -4231,7 +4253,7 @@
       <c r="AE4" s="13"/>
       <c r="AF4" s="15"/>
     </row>
-    <row r="5" spans="1:32" s="19" customFormat="1" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="34">
         <v>2</v>
       </c>
@@ -4315,7 +4337,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:32" s="19" customFormat="1" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="32">
         <v>3</v>
       </c>
@@ -4398,7 +4420,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="34">
         <v>4</v>
       </c>
@@ -4482,7 +4504,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="32">
         <v>5</v>
       </c>
@@ -4566,12 +4588,16 @@
       <c r="AE8" s="13"/>
       <c r="AF8" s="15"/>
     </row>
-    <row r="9" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="32">
         <v>6</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="79">
+        <v>2.6987899999999998</v>
+      </c>
+      <c r="C9" s="73">
+        <v>2.74492</v>
+      </c>
       <c r="D9" s="65">
         <v>42551</v>
       </c>
@@ -4650,12 +4676,16 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="32">
         <v>7</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="79">
+        <v>2.7037900000000001</v>
+      </c>
+      <c r="C10" s="73">
+        <v>2.74492</v>
+      </c>
       <c r="D10" s="65">
         <v>42551</v>
       </c>
@@ -4734,12 +4764,16 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="32">
         <v>8</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="79">
+        <v>2.7107899999999998</v>
+      </c>
+      <c r="C11" s="73">
+        <v>2.74492</v>
+      </c>
       <c r="D11" s="65">
         <v>42551</v>
       </c>
@@ -4820,12 +4854,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
         <v>9</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="73"/>
+      <c r="B12" s="79">
+        <v>2.7107899999999998</v>
+      </c>
+      <c r="C12" s="73">
+        <v>2.76492</v>
+      </c>
       <c r="D12" s="65">
         <v>42551</v>
       </c>
@@ -4908,12 +4946,16 @@
       </c>
       <c r="AF12" s="15"/>
     </row>
-    <row r="13" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <v>10</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="79">
+        <v>2.7107899999999998</v>
+      </c>
+      <c r="C13" s="73">
+        <v>2.76492</v>
+      </c>
       <c r="D13" s="66">
         <v>42551</v>
       </c>
@@ -4990,12 +5032,16 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="32">
         <v>11</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="79">
+        <v>2.7107899999999998</v>
+      </c>
+      <c r="C14" s="73">
+        <v>2.7599200000000002</v>
+      </c>
       <c r="D14" s="65">
         <v>42551</v>
       </c>
@@ -5076,7 +5122,7 @@
       <c r="AE14" s="15"/>
       <c r="AF14" s="15"/>
     </row>
-    <row r="15" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
         <v>12</v>
       </c>
@@ -5164,7 +5210,7 @@
       <c r="AE15" s="48"/>
       <c r="AF15" s="15"/>
     </row>
-    <row r="16" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="32">
         <v>13</v>
       </c>
@@ -5252,7 +5298,7 @@
       <c r="AE16" s="48"/>
       <c r="AF16" s="15"/>
     </row>
-    <row r="17" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="32">
         <v>14</v>
       </c>
@@ -5348,7 +5394,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="32">
         <v>15</v>
       </c>
@@ -5444,7 +5490,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="32">
         <v>16</v>
       </c>
@@ -5532,7 +5578,7 @@
       <c r="AE19" s="58"/>
       <c r="AF19" s="58"/>
     </row>
-    <row r="20" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
         <v>17</v>
       </c>
@@ -5624,7 +5670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="31.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="32">
         <v>18</v>
       </c>
@@ -5708,7 +5754,7 @@
       <c r="AE21" s="15"/>
       <c r="AF21" s="15"/>
     </row>
-    <row r="22" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="32">
         <v>20</v>
       </c>
@@ -5794,7 +5840,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="32">
         <v>21</v>
       </c>
@@ -5879,7 +5925,7 @@
       <c r="AE23" s="15"/>
       <c r="AF23" s="15"/>
     </row>
-    <row r="24" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="32">
         <v>22</v>
       </c>
@@ -5891,7 +5937,7 @@
         <v>2.738</v>
       </c>
       <c r="D24" s="65">
-        <f t="shared" ref="D24:D37" si="0">D23</f>
+        <f>D23</f>
         <v>42558</v>
       </c>
       <c r="E24" s="13" t="s">
@@ -5965,7 +6011,7 @@
       <c r="AE24" s="15"/>
       <c r="AF24" s="15"/>
     </row>
-    <row r="25" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="32">
         <v>23</v>
       </c>
@@ -5973,11 +6019,11 @@
         <v>99</v>
       </c>
       <c r="C25" s="73">
-        <f t="shared" ref="C25:C36" si="1">C24-0.001</f>
+        <f>C24-0.001</f>
         <v>2.7370000000000001</v>
       </c>
       <c r="D25" s="65">
-        <f t="shared" si="0"/>
+        <f>D24</f>
         <v>42558</v>
       </c>
       <c r="E25" s="13" t="s">
@@ -6049,108 +6095,101 @@
       <c r="AC25" s="15"/>
       <c r="AD25" s="15"/>
       <c r="AE25" s="15"/>
+      <c r="AF25" s="112"/>
     </row>
-    <row r="26" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A26" s="32">
+        <f>A25+1</f>
         <v>24</v>
       </c>
-      <c r="B26" s="79" t="s">
-        <v>99</v>
+      <c r="B26" s="79">
+        <v>2.7669999999999999</v>
       </c>
       <c r="C26" s="73">
-        <v>2.7370000000000001</v>
-      </c>
-      <c r="D26" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C25+0.001</f>
+        <v>2.738</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>109</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G26" s="13">
-        <v>5</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="13">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I26" s="14">
+        <v>60</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K26" s="13">
-        <v>200</v>
-      </c>
-      <c r="L26" s="13">
-        <v>0.72</v>
-      </c>
-      <c r="M26" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="N26" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O26" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P26" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13">
+      <c r="K26" s="14">
+        <v>1</v>
+      </c>
+      <c r="L26" s="14">
+        <v>0.54</v>
+      </c>
+      <c r="M26" s="15">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N26" s="15"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13">
+      <c r="S26" s="15"/>
+      <c r="T26" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13">
+      <c r="U26" s="15"/>
+      <c r="V26" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13">
+      <c r="W26" s="15"/>
+      <c r="X26" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13">
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA26" s="13"/>
-      <c r="AB26" s="13">
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC26" s="15"/>
       <c r="AD26" s="15"/>
       <c r="AE26" s="15"/>
-      <c r="AF26" t="s">
-        <v>105</v>
-      </c>
+      <c r="AF26" s="109"/>
     </row>
-    <row r="27" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="32">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="79" t="s">
         <v>99</v>
       </c>
       <c r="C27" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7360000000000002</v>
-      </c>
-      <c r="D27" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="D27" s="65" t="str">
+        <f>D26</f>
+        <v>11-juil</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>20</v>
@@ -6162,7 +6201,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
@@ -6174,7 +6213,7 @@
         <v>200</v>
       </c>
       <c r="L27" s="13">
-        <v>0.70299999999999996</v>
+        <v>0.72</v>
       </c>
       <c r="M27" s="13">
         <v>0.01</v>
@@ -6193,12 +6232,10 @@
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S27" s="13">
-        <v>3</v>
-      </c>
+      <c r="S27" s="13"/>
       <c r="T27" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U27" s="13"/>
       <c r="V27" s="13">
@@ -6223,110 +6260,104 @@
       <c r="AC27" s="15"/>
       <c r="AD27" s="15"/>
       <c r="AE27" s="15"/>
-      <c r="AF27" s="15"/>
+      <c r="AF27" s="108" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="32">
-        <v>26</v>
-      </c>
-      <c r="B28" s="79" t="s">
-        <v>99</v>
+        <f>A27+1</f>
+        <v>25</v>
+      </c>
+      <c r="B28" s="79">
+        <v>2.7669999999999999</v>
       </c>
       <c r="C28" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7350000000000003</v>
-      </c>
-      <c r="D28" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C27+0.001</f>
+        <v>2.738</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>109</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G28" s="13">
-        <v>5</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" s="13">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="14">
+        <v>30</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K28" s="13">
-        <v>200</v>
-      </c>
-      <c r="L28" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="M28" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N28" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O28" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P28" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13">
+      <c r="K28" s="14">
+        <v>2</v>
+      </c>
+      <c r="L28" s="14">
+        <v>0.52</v>
+      </c>
+      <c r="M28" s="15">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N28" s="15"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13">
+      <c r="S28" s="15"/>
+      <c r="T28" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13">
+      <c r="U28" s="15"/>
+      <c r="V28" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13">
+      <c r="W28" s="15"/>
+      <c r="X28" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13">
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA28" s="13"/>
-      <c r="AB28" s="13">
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC28" s="15"/>
       <c r="AD28" s="15"/>
       <c r="AE28" s="15"/>
-      <c r="AF28" t="s">
-        <v>104</v>
-      </c>
+      <c r="AF28" s="109"/>
     </row>
-    <row r="29" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="32">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="79" t="s">
         <v>99</v>
       </c>
       <c r="C29" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7340000000000004</v>
-      </c>
-      <c r="D29" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C28-0.001</f>
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="D29" s="65" t="str">
+        <f>D28</f>
+        <v>11-juil</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>20</v>
@@ -6338,7 +6369,7 @@
         <v>5</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I29" s="13">
         <v>1</v>
@@ -6350,7 +6381,7 @@
         <v>200</v>
       </c>
       <c r="L29" s="13">
-        <v>0.68</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="M29" s="13">
         <v>0.01</v>
@@ -6369,10 +6400,12 @@
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S29" s="13"/>
+      <c r="S29" s="13">
+        <v>3</v>
+      </c>
       <c r="T29" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U29" s="13"/>
       <c r="V29" s="13">
@@ -6399,84 +6432,78 @@
       <c r="AE29" s="15"/>
       <c r="AF29" s="15"/>
     </row>
-    <row r="30" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="33">
-        <v>28</v>
-      </c>
-      <c r="B30" s="79" t="s">
-        <v>99</v>
+        <f>A29+1</f>
+        <v>26</v>
+      </c>
+      <c r="B30" s="79">
+        <v>2.7669999999999999</v>
       </c>
       <c r="C30" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7330000000000005</v>
-      </c>
-      <c r="D30" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C29+0.001</f>
+        <v>2.738</v>
+      </c>
+      <c r="D30" s="63" t="s">
+        <v>109</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G30" s="13">
-        <v>5</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I30" s="13">
+        <v>10</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="14">
         <v>20</v>
       </c>
       <c r="J30" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K30" s="13">
-        <v>20</v>
-      </c>
-      <c r="L30" s="13">
-        <v>0.64</v>
-      </c>
-      <c r="M30" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="N30" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O30" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P30" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13">
+      <c r="K30" s="14">
+        <v>3</v>
+      </c>
+      <c r="L30" s="14">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="M30" s="15">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N30" s="15"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13">
+      <c r="S30" s="15"/>
+      <c r="T30" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U30" s="13"/>
-      <c r="V30" s="13">
+      <c r="U30" s="15"/>
+      <c r="V30" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W30" s="13"/>
-      <c r="X30" s="13">
+      <c r="W30" s="15"/>
+      <c r="X30" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13">
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA30" s="13"/>
-      <c r="AB30" s="13">
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
@@ -6485,20 +6512,20 @@
       <c r="AE30" s="15"/>
       <c r="AF30" s="15"/>
     </row>
-    <row r="31" spans="1:32" s="51" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" s="51" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A31" s="33">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" s="79" t="s">
         <v>99</v>
       </c>
       <c r="C31" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7320000000000007</v>
-      </c>
-      <c r="D31" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C30-0.001</f>
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="D31" s="65" t="str">
+        <f>D30</f>
+        <v>11-juil</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>20</v>
@@ -6510,22 +6537,22 @@
         <v>5</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I31" s="13">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>94</v>
       </c>
       <c r="K31" s="13">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="L31" s="43">
-        <v>0.64300000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="M31" s="13">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N31" s="13">
         <v>30000</v>
@@ -6569,171 +6596,161 @@
       <c r="AC31" s="28"/>
       <c r="AD31" s="28"/>
       <c r="AE31" s="28"/>
-      <c r="AF31" s="28"/>
+      <c r="AF31" s="119" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="32" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="33">
-        <v>30</v>
-      </c>
-      <c r="B32" s="79" t="s">
-        <v>99</v>
+        <f>A31+1</f>
+        <v>27</v>
+      </c>
+      <c r="B32" s="79">
+        <v>2.7669999999999999</v>
       </c>
       <c r="C32" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7310000000000008</v>
-      </c>
-      <c r="D32" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C31+0.001</f>
+        <v>2.738</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>109</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G32" s="13">
-        <v>5</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="13">
         <v>10</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I32" s="14">
+        <v>15</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="13">
-        <v>20</v>
-      </c>
-      <c r="L32" s="43">
-        <v>0.59</v>
-      </c>
-      <c r="M32" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="N32" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O32" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P32" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43">
+      <c r="K32" s="14">
+        <v>4</v>
+      </c>
+      <c r="L32" s="106">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="M32" s="15">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N32" s="15"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S32" s="43"/>
-      <c r="T32" s="43">
+      <c r="S32" s="28"/>
+      <c r="T32" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U32" s="43"/>
-      <c r="V32" s="43">
+      <c r="U32" s="28"/>
+      <c r="V32" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W32" s="43"/>
-      <c r="X32" s="43">
+      <c r="W32" s="28"/>
+      <c r="X32" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="43">
+      <c r="Y32" s="28"/>
+      <c r="Z32" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA32" s="43"/>
-      <c r="AB32" s="43">
+      <c r="AA32" s="28"/>
+      <c r="AB32" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC32" s="28"/>
       <c r="AD32" s="28"/>
       <c r="AE32" s="28"/>
+      <c r="AF32" s="109"/>
     </row>
-    <row r="33" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="33">
-        <v>31</v>
-      </c>
-      <c r="B33" s="79" t="s">
-        <v>99</v>
+        <f>A32+1</f>
+        <v>28</v>
+      </c>
+      <c r="B33" s="79">
+        <v>2.7669999999999999</v>
       </c>
       <c r="C33" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7300000000000009</v>
-      </c>
-      <c r="D33" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <v>2.274</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>109</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G33" s="13">
-        <v>5</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="43">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="H33" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="I33" s="106">
+        <v>1</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K33" s="43">
+      <c r="K33" s="106">
         <v>10</v>
       </c>
-      <c r="L33" s="43">
-        <v>0.68200000000000005</v>
-      </c>
-      <c r="M33" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="N33" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O33" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P33" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43">
+      <c r="L33" s="106">
+        <v>0.59</v>
+      </c>
+      <c r="M33" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="N33" s="15"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S33" s="43"/>
-      <c r="T33" s="43">
+      <c r="S33" s="28"/>
+      <c r="T33" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U33" s="43"/>
-      <c r="V33" s="43">
+      <c r="U33" s="28"/>
+      <c r="V33" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W33" s="43"/>
-      <c r="X33" s="43">
+      <c r="W33" s="28"/>
+      <c r="X33" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y33" s="43"/>
-      <c r="Z33" s="43">
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA33" s="43"/>
-      <c r="AB33" s="43">
+      <c r="AA33" s="28"/>
+      <c r="AB33" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
@@ -6742,20 +6759,20 @@
       <c r="AE33" s="28"/>
       <c r="AF33" s="28"/>
     </row>
-    <row r="34" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="33">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B34" s="79" t="s">
         <v>99</v>
       </c>
       <c r="C34" s="73">
-        <f t="shared" si="1"/>
-        <v>2.729000000000001</v>
-      </c>
-      <c r="D34" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C33-0.001</f>
+        <v>2.2730000000000001</v>
+      </c>
+      <c r="D34" s="65" t="str">
+        <f>D33</f>
+        <v>11-juil</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>20</v>
@@ -6770,16 +6787,16 @@
         <v>103</v>
       </c>
       <c r="I34" s="43">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J34" s="13" t="s">
         <v>94</v>
       </c>
       <c r="K34" s="43">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="L34" s="43">
-        <v>0.59699999999999998</v>
+        <v>0.68</v>
       </c>
       <c r="M34" s="13">
         <v>0.01</v>
@@ -6828,84 +6845,78 @@
       <c r="AE34" s="28"/>
       <c r="AF34" s="28"/>
     </row>
-    <row r="35" spans="1:32" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="33">
-        <v>33</v>
-      </c>
-      <c r="B35" s="79" t="s">
-        <v>99</v>
+        <f>A34+1</f>
+        <v>28</v>
+      </c>
+      <c r="B35" s="79">
+        <v>2.7669999999999999</v>
       </c>
       <c r="C35" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7280000000000011</v>
-      </c>
-      <c r="D35" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C34+0.001</f>
+        <v>2.274</v>
+      </c>
+      <c r="D35" s="63" t="s">
+        <v>109</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G35" s="13">
-        <v>5</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I35" s="43">
-        <v>6.6666699999999999</v>
+        <v>10</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I35" s="106">
+        <v>12</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K35" s="43">
-        <v>30</v>
-      </c>
-      <c r="L35" s="43">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="M35" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="N35" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O35" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P35" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43">
+      <c r="K35" s="106">
+        <v>5</v>
+      </c>
+      <c r="L35" s="106">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="M35" s="15">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N35" s="15"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S35" s="43"/>
-      <c r="T35" s="43">
+      <c r="S35" s="28"/>
+      <c r="T35" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U35" s="43"/>
-      <c r="V35" s="43">
+      <c r="U35" s="28"/>
+      <c r="V35" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W35" s="43"/>
-      <c r="X35" s="43">
+      <c r="W35" s="28"/>
+      <c r="X35" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="43">
+      <c r="Y35" s="28"/>
+      <c r="Z35" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA35" s="43"/>
-      <c r="AB35" s="43">
+      <c r="AA35" s="28"/>
+      <c r="AB35" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
@@ -6914,105 +6925,87 @@
       <c r="AE35" s="28"/>
       <c r="AF35" s="28"/>
     </row>
-    <row r="36" spans="1:32" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="33">
-        <v>34</v>
-      </c>
-      <c r="B36" s="79" t="s">
+    <row r="36" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="91">
+        <f>A35+1</f>
+        <v>29</v>
+      </c>
+      <c r="B36" s="113"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="85" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="85">
+        <v>10</v>
+      </c>
+      <c r="H36" s="87"/>
+      <c r="I36" s="116"/>
+      <c r="J36" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="K36" s="116"/>
+      <c r="L36" s="116"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="87"/>
+      <c r="O36" s="92"/>
+      <c r="P36" s="87"/>
+      <c r="Q36" s="116"/>
+      <c r="R36" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="116"/>
+      <c r="T36" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="U36" s="116"/>
+      <c r="V36" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="W36" s="116"/>
+      <c r="X36" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="116"/>
+      <c r="Z36" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AA36" s="116"/>
+      <c r="AB36" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AC36" s="116"/>
+      <c r="AD36" s="116"/>
+      <c r="AE36" s="116"/>
+      <c r="AF36" s="116" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="33">
+        <v>28</v>
+      </c>
+      <c r="B37" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="73">
-        <f t="shared" si="1"/>
-        <v>2.7270000000000012</v>
-      </c>
-      <c r="D36" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="13">
-        <v>5</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I36" s="43">
-        <v>4</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="K36" s="43">
-        <v>50</v>
-      </c>
-      <c r="L36" s="43">
-        <v>0.52600000000000002</v>
-      </c>
-      <c r="M36" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="N36" s="13">
-        <v>30000</v>
-      </c>
-      <c r="O36" s="39">
-        <v>2000</v>
-      </c>
-      <c r="P36" s="13">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q36" s="43"/>
-      <c r="R36" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="S36" s="43"/>
-      <c r="T36" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="U36" s="43"/>
-      <c r="V36" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="W36" s="43"/>
-      <c r="X36" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="Y36" s="43"/>
-      <c r="Z36" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AA36" s="43"/>
-      <c r="AB36" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AC36" s="28"/>
-      <c r="AD36" s="28"/>
-      <c r="AE36" s="28"/>
-      <c r="AF36" s="28"/>
-    </row>
-    <row r="37" spans="1:32" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="33">
-        <v>35</v>
-      </c>
-      <c r="B37" s="80">
-        <v>2.4900000000000002</v>
-      </c>
       <c r="C37" s="74">
-        <v>2.72</v>
-      </c>
-      <c r="D37" s="65">
-        <f t="shared" si="0"/>
-        <v>42558</v>
+        <f>C36-0.001</f>
+        <v>-1E-3</v>
+      </c>
+      <c r="D37" s="65" t="str">
+        <f>D36</f>
+        <v>11-juil</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>20</v>
@@ -7024,10 +7017,10 @@
         <v>5</v>
       </c>
       <c r="H37" s="43" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="I37" s="43">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J37" s="13" t="s">
         <v>94</v>
@@ -7036,16 +7029,16 @@
         <v>20</v>
       </c>
       <c r="L37" s="43">
-        <v>0.51200000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="M37" s="13">
         <v>0.01</v>
       </c>
       <c r="N37" s="43">
-        <v>7000</v>
+        <v>30000</v>
       </c>
       <c r="O37" s="45">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="P37" s="13">
         <v>3.2000000000000002E-3</v>
@@ -7085,19 +7078,20 @@
       <c r="AE37" s="28"/>
       <c r="AF37" s="28"/>
     </row>
-    <row r="38" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A38" s="33">
         <f>A37+1</f>
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B38" s="80">
-        <v>2.7309999999999999</v>
+        <v>2.7669999999999999</v>
       </c>
       <c r="C38" s="74">
-        <v>2.7120000000000002</v>
-      </c>
-      <c r="D38" s="68" t="s">
-        <v>106</v>
+        <f>C37+0.001</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="105" t="s">
+        <v>109</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>107</v>
@@ -7108,54 +7102,54 @@
       <c r="G38" s="43">
         <v>10</v>
       </c>
-      <c r="H38" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="I38" s="43">
-        <v>1</v>
+      <c r="H38" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="I38" s="106">
+        <v>6</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K38" s="43">
-        <v>20</v>
-      </c>
-      <c r="L38" s="43">
-        <v>7.27</v>
-      </c>
-      <c r="M38" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="N38" s="43"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="43"/>
-      <c r="R38" s="43">
+        <v>94</v>
+      </c>
+      <c r="K38" s="106">
+        <v>10</v>
+      </c>
+      <c r="L38" s="106">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="M38" s="28">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N38" s="28"/>
+      <c r="O38" s="111"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S38" s="43"/>
-      <c r="T38" s="43">
+      <c r="S38" s="28"/>
+      <c r="T38" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U38" s="43"/>
-      <c r="V38" s="43">
+      <c r="U38" s="28"/>
+      <c r="V38" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W38" s="43"/>
-      <c r="X38" s="43">
+      <c r="W38" s="28"/>
+      <c r="X38" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y38" s="43"/>
-      <c r="Z38" s="43">
+      <c r="Y38" s="28"/>
+      <c r="Z38" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA38" s="43"/>
-      <c r="AB38" s="43">
+      <c r="AA38" s="28"/>
+      <c r="AB38" s="107">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
@@ -7164,158 +7158,151 @@
       <c r="AE38" s="28"/>
       <c r="AF38" s="28"/>
     </row>
-    <row r="39" spans="1:32" ht="48" x14ac:dyDescent="0.2">
-      <c r="A39" s="33">
-        <f t="shared" ref="A39:A60" si="2">A38+1</f>
-        <v>37</v>
-      </c>
-      <c r="B39" s="80">
-        <v>2.7309999999999999</v>
-      </c>
-      <c r="C39" s="74">
-        <f>C38+0.001</f>
-        <v>2.7130000000000001</v>
-      </c>
-      <c r="D39" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="E39" s="13" t="s">
+    <row r="39" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="91">
+        <f>A38+1</f>
+        <v>30</v>
+      </c>
+      <c r="B39" s="82"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="110" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="43">
+      <c r="G39" s="86">
         <v>10</v>
       </c>
-      <c r="H39" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="I39" s="43">
-        <v>1</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K39" s="43">
+      <c r="H39" s="116"/>
+      <c r="I39" s="116"/>
+      <c r="J39" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" s="116"/>
+      <c r="L39" s="116"/>
+      <c r="M39" s="116"/>
+      <c r="N39" s="116"/>
+      <c r="O39" s="117"/>
+      <c r="P39" s="87"/>
+      <c r="Q39" s="116"/>
+      <c r="R39" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="116"/>
+      <c r="T39" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="116"/>
+      <c r="V39" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="116"/>
+      <c r="X39" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="116"/>
+      <c r="Z39" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="116"/>
+      <c r="AB39" s="118">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="116"/>
+      <c r="AD39" s="116"/>
+      <c r="AE39" s="116"/>
+      <c r="AF39" s="116" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="33">
+        <v>29</v>
+      </c>
+      <c r="B40" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="74">
+        <f>C39-0.001</f>
+        <v>-1E-3</v>
+      </c>
+      <c r="D40" s="68" t="str">
+        <f>D39</f>
+        <v>11-juil</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="L39" s="43">
-        <v>7.0350000000000001</v>
-      </c>
-      <c r="M39" s="43">
-        <v>0.1</v>
-      </c>
-      <c r="N39" s="43"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="43"/>
-      <c r="R39" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="S39" s="43"/>
-      <c r="T39" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="U39" s="43"/>
-      <c r="V39" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="W39" s="43"/>
-      <c r="X39" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="Y39" s="43"/>
-      <c r="Z39" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AA39" s="43"/>
-      <c r="AB39" s="43">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
-      <c r="AF39" s="28"/>
-    </row>
-    <row r="40" spans="1:32" ht="48" x14ac:dyDescent="0.2">
-      <c r="A40" s="33">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="B40" s="80">
-        <v>2.7309999999999999</v>
-      </c>
-      <c r="C40" s="74">
-        <f t="shared" ref="C40:C43" si="3">C39+0.001</f>
-        <v>2.714</v>
-      </c>
-      <c r="D40" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G40" s="43">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="I40" s="14">
+        <v>103</v>
+      </c>
+      <c r="I40" s="13">
+        <v>200</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="K40" s="13">
         <v>1</v>
       </c>
-      <c r="J40" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K40" s="14">
-        <v>20</v>
-      </c>
-      <c r="L40" s="14">
-        <v>7.2149999999999999</v>
-      </c>
-      <c r="M40" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="N40" s="15"/>
-      <c r="O40" s="55"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="35">
+      <c r="L40" s="13">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="M40" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N40" s="13">
+        <v>30000</v>
+      </c>
+      <c r="O40" s="39">
+        <v>2000</v>
+      </c>
+      <c r="P40" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S40" s="15"/>
-      <c r="T40" s="35">
+      <c r="S40" s="13"/>
+      <c r="T40" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U40" s="15"/>
-      <c r="V40" s="35">
+      <c r="U40" s="13"/>
+      <c r="V40" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W40" s="15"/>
-      <c r="X40" s="35">
+      <c r="W40" s="13"/>
+      <c r="X40" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="35">
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA40" s="15"/>
-      <c r="AB40" s="35">
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
@@ -7324,20 +7311,20 @@
       <c r="AE40" s="28"/>
       <c r="AF40" s="15"/>
     </row>
-    <row r="41" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A41" s="33">
-        <f t="shared" si="2"/>
-        <v>39</v>
+        <f>A40+1</f>
+        <v>30</v>
       </c>
       <c r="B41" s="80">
-        <v>2.7309999999999999</v>
+        <v>2.7669999999999999</v>
       </c>
       <c r="C41" s="74">
-        <f t="shared" si="3"/>
-        <v>2.7149999999999999</v>
-      </c>
-      <c r="D41" s="68" t="s">
-        <v>106</v>
+        <f>C40+0.001</f>
+        <v>0</v>
+      </c>
+      <c r="D41" s="105" t="s">
+        <v>109</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>107</v>
@@ -7348,23 +7335,23 @@
       <c r="G41" s="43">
         <v>10</v>
       </c>
-      <c r="H41" s="13" t="s">
-        <v>103</v>
+      <c r="H41" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="I41" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="K41" s="14">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="L41" s="14">
-        <v>7.2229999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="M41" s="15">
-        <v>0.05</v>
+        <v>3.3329999999999999E-2</v>
       </c>
       <c r="N41" s="15"/>
       <c r="O41" s="55"/>
@@ -7400,184 +7387,177 @@
         <v>0</v>
       </c>
       <c r="AC41" s="15"/>
-      <c r="AD41" s="92"/>
-      <c r="AE41" s="92"/>
+      <c r="AD41" s="90"/>
+      <c r="AE41" s="90"/>
       <c r="AF41" s="15"/>
     </row>
-    <row r="42" spans="1:32" ht="48" x14ac:dyDescent="0.2">
-      <c r="A42" s="33">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="B42" s="80">
-        <v>2.7309999999999999</v>
-      </c>
-      <c r="C42" s="74">
-        <f t="shared" si="3"/>
-        <v>2.7159999999999997</v>
-      </c>
-      <c r="D42" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="13" t="s">
+    <row r="42" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="91">
+        <f>A41+1</f>
+        <v>31</v>
+      </c>
+      <c r="B42" s="82"/>
+      <c r="C42" s="83"/>
+      <c r="D42" s="110" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="43">
+      <c r="G42" s="86">
         <v>10</v>
       </c>
-      <c r="H42" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I42" s="14">
-        <v>2</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K42" s="14">
-        <v>1000</v>
-      </c>
-      <c r="L42" s="14">
-        <v>7.1159999999999997</v>
-      </c>
-      <c r="M42" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="N42" s="15"/>
-      <c r="O42" s="55"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="35">
+      <c r="H42" s="87"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="K42" s="87"/>
+      <c r="L42" s="87"/>
+      <c r="M42" s="87"/>
+      <c r="N42" s="87"/>
+      <c r="O42" s="92"/>
+      <c r="P42" s="87"/>
+      <c r="Q42" s="87"/>
+      <c r="R42" s="93">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S42" s="15"/>
-      <c r="T42" s="35">
+      <c r="S42" s="87"/>
+      <c r="T42" s="93">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U42" s="15"/>
-      <c r="V42" s="35">
+      <c r="U42" s="87"/>
+      <c r="V42" s="93">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W42" s="15"/>
-      <c r="X42" s="35">
+      <c r="W42" s="87"/>
+      <c r="X42" s="93">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y42" s="15"/>
-      <c r="Z42" s="35">
+      <c r="Y42" s="87"/>
+      <c r="Z42" s="93">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA42" s="15"/>
-      <c r="AB42" s="35">
+      <c r="AA42" s="87"/>
+      <c r="AB42" s="93">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AC42" s="15"/>
-      <c r="AD42" s="92"/>
-      <c r="AE42" s="92"/>
-      <c r="AF42" s="15"/>
+      <c r="AC42" s="87"/>
+      <c r="AD42" s="94"/>
+      <c r="AE42" s="94"/>
+      <c r="AF42" s="87" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="43" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A43" s="33">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-      <c r="B43" s="80">
-        <v>2.7309999999999999</v>
+        <v>30</v>
+      </c>
+      <c r="B43" s="80" t="s">
+        <v>99</v>
       </c>
       <c r="C43" s="74">
-        <f t="shared" si="3"/>
-        <v>2.7169999999999996</v>
-      </c>
-      <c r="D43" s="68" t="s">
-        <v>106</v>
+        <f>C42-0.001</f>
+        <v>-1E-3</v>
+      </c>
+      <c r="D43" s="68" t="str">
+        <f>D42</f>
+        <v>11-juil</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="F43" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G43" s="43">
+        <v>5</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" s="13">
         <v>10</v>
       </c>
-      <c r="H43" s="81" t="s">
-        <v>108</v>
-      </c>
-      <c r="I43" s="14">
-        <v>2</v>
-      </c>
       <c r="J43" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="K43" s="14">
-        <v>1000</v>
-      </c>
-      <c r="L43" s="14">
-        <v>7.2009999999999996</v>
-      </c>
-      <c r="M43" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="N43" s="15"/>
-      <c r="O43" s="55"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="35">
+        <v>94</v>
+      </c>
+      <c r="K43" s="13">
+        <v>20</v>
+      </c>
+      <c r="L43" s="13">
+        <v>0.59</v>
+      </c>
+      <c r="M43" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N43" s="13">
+        <v>30000</v>
+      </c>
+      <c r="O43" s="39">
+        <v>2000</v>
+      </c>
+      <c r="P43" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S43" s="15"/>
-      <c r="T43" s="35">
+      <c r="S43" s="13"/>
+      <c r="T43" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U43" s="15"/>
-      <c r="V43" s="35">
+      <c r="U43" s="13"/>
+      <c r="V43" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W43" s="15"/>
-      <c r="X43" s="35">
+      <c r="W43" s="13"/>
+      <c r="X43" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="35">
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="35">
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC43" s="15"/>
-      <c r="AD43" s="92"/>
-      <c r="AE43" s="92"/>
-      <c r="AF43" s="15"/>
+      <c r="AD43" s="90"/>
+      <c r="AE43" s="90"/>
+      <c r="AF43" s="108"/>
     </row>
-    <row r="44" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A44" s="33">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f>A43+1</f>
+        <v>31</v>
       </c>
       <c r="B44" s="80">
-        <v>2.7320000000000002</v>
+        <v>2.7669999999999999</v>
       </c>
       <c r="C44" s="74">
-        <f>C43</f>
-        <v>2.7169999999999996</v>
-      </c>
-      <c r="D44" s="68" t="s">
-        <v>106</v>
+        <f>C43+0.001</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="105" t="s">
+        <v>109</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>107</v>
@@ -7588,23 +7568,23 @@
       <c r="G44" s="43">
         <v>10</v>
       </c>
-      <c r="H44" s="81" t="s">
-        <v>108</v>
+      <c r="H44" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="I44" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="K44" s="14">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L44" s="14">
-        <v>7.109</v>
+        <v>0.5</v>
       </c>
       <c r="M44" s="15">
-        <v>0.2</v>
+        <v>3.3329999999999999E-2</v>
       </c>
       <c r="N44" s="15"/>
       <c r="O44" s="55"/>
@@ -7640,224 +7620,270 @@
         <v>0</v>
       </c>
       <c r="AC44" s="15"/>
-      <c r="AD44" s="92"/>
-      <c r="AE44" s="92"/>
+      <c r="AD44" s="90"/>
+      <c r="AE44" s="90"/>
       <c r="AF44" s="15"/>
     </row>
-    <row r="45" spans="1:32" s="106" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" s="102">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="B45" s="82"/>
-      <c r="C45" s="83"/>
-      <c r="D45" s="84" t="s">
+    <row r="45" spans="1:32" s="95" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="33">
+        <f>A44+1</f>
+        <v>32</v>
+      </c>
+      <c r="B45" s="80">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C45" s="74">
+        <f>C44+0.001</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D45" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="43">
+        <v>10</v>
+      </c>
+      <c r="H45" s="81" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="14">
+        <v>2</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K45" s="14">
+        <v>1000</v>
+      </c>
+      <c r="L45" s="14">
+        <v>7.2009999999999996</v>
+      </c>
+      <c r="M45" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="N45" s="15"/>
+      <c r="O45" s="55"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="35">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="S45" s="15"/>
+      <c r="T45" s="35">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="U45" s="15"/>
+      <c r="V45" s="35">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="W45" s="15"/>
+      <c r="X45" s="35">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="35">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AA45" s="15"/>
+      <c r="AB45" s="35">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AC45" s="15"/>
+      <c r="AD45" s="90"/>
+      <c r="AE45" s="90"/>
+      <c r="AF45" s="15"/>
+    </row>
+    <row r="46" spans="1:32" s="95" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="33">
+        <v>31</v>
+      </c>
+      <c r="B46" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="88">
+        <f>C45-0.001</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="65" t="str">
+        <f>D45</f>
+        <v>8-juil.</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="43">
+        <v>5</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I46" s="13">
+        <v>20</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="K46" s="13">
+        <v>10</v>
+      </c>
+      <c r="L46" s="13">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="M46" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N46" s="13">
+        <v>30000</v>
+      </c>
+      <c r="O46" s="39">
+        <v>2000</v>
+      </c>
+      <c r="P46" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="W46" s="13"/>
+      <c r="X46" s="13">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="13">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13">
+        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
+        <v>0</v>
+      </c>
+      <c r="AC46" s="15"/>
+      <c r="AD46" s="90"/>
+      <c r="AE46" s="90"/>
+      <c r="AF46" s="15"/>
+    </row>
+    <row r="47" spans="1:32" s="95" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="33">
+        <f>A46+1</f>
+        <v>32</v>
+      </c>
+      <c r="B47" s="89">
+        <v>2.7669999999999999</v>
+      </c>
+      <c r="C47" s="88">
+        <f>C46+0.001</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D47" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="E45" s="85" t="s">
+      <c r="E47" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="F45" s="85" t="s">
+      <c r="F47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G45" s="86">
+      <c r="G47" s="43">
         <v>10</v>
       </c>
-      <c r="H45" s="87"/>
-      <c r="I45" s="87"/>
-      <c r="J45" s="85" t="s">
+      <c r="H47" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I47" s="14">
+        <v>2</v>
+      </c>
+      <c r="J47" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K45" s="87"/>
-      <c r="L45" s="87"/>
-      <c r="M45" s="87"/>
-      <c r="N45" s="87"/>
-      <c r="O45" s="103"/>
-      <c r="P45" s="87"/>
-      <c r="Q45" s="87"/>
-      <c r="R45" s="104">
+      <c r="K47" s="14">
+        <v>30</v>
+      </c>
+      <c r="L47" s="14">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="M47" s="15">
+        <v>3.3329999999999999E-2</v>
+      </c>
+      <c r="N47" s="15"/>
+      <c r="O47" s="55"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S45" s="87"/>
-      <c r="T45" s="104">
+      <c r="S47" s="15"/>
+      <c r="T47" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U45" s="87"/>
-      <c r="V45" s="104">
+      <c r="U47" s="15"/>
+      <c r="V47" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W45" s="87"/>
-      <c r="X45" s="104">
+      <c r="W47" s="15"/>
+      <c r="X47" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y45" s="87"/>
-      <c r="Z45" s="104">
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA45" s="87"/>
-      <c r="AB45" s="104">
+      <c r="AA47" s="15"/>
+      <c r="AB47" s="35">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AC45" s="87"/>
-      <c r="AD45" s="105"/>
-      <c r="AE45" s="105"/>
-      <c r="AF45" s="87" t="s">
-        <v>112</v>
-      </c>
+      <c r="AC47" s="15"/>
+      <c r="AD47" s="90"/>
+      <c r="AE47" s="90"/>
+      <c r="AF47" s="15"/>
     </row>
-    <row r="46" spans="1:32" s="106" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A46" s="102">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="B46" s="88"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="84" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" s="85" t="s">
-        <v>21</v>
-      </c>
-      <c r="G46" s="86">
-        <v>10</v>
-      </c>
-      <c r="H46" s="87"/>
-      <c r="I46" s="87"/>
-      <c r="J46" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="K46" s="87"/>
-      <c r="L46" s="87"/>
-      <c r="M46" s="87"/>
-      <c r="N46" s="87"/>
-      <c r="O46" s="103"/>
-      <c r="P46" s="87"/>
-      <c r="Q46" s="87"/>
-      <c r="R46" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="S46" s="87"/>
-      <c r="T46" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="U46" s="87"/>
-      <c r="V46" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="W46" s="87"/>
-      <c r="X46" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="Y46" s="87"/>
-      <c r="Z46" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AA46" s="87"/>
-      <c r="AB46" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="87"/>
-      <c r="AD46" s="105"/>
-      <c r="AE46" s="105"/>
-      <c r="AF46" s="87" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:32" s="106" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A47" s="102">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="B47" s="88"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="84" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="85" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" s="86">
-        <v>10</v>
-      </c>
-      <c r="H47" s="87"/>
-      <c r="I47" s="87"/>
-      <c r="J47" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
-      <c r="M47" s="87"/>
-      <c r="N47" s="87"/>
-      <c r="O47" s="103"/>
-      <c r="P47" s="87"/>
-      <c r="Q47" s="87"/>
-      <c r="R47" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="S47" s="87"/>
-      <c r="T47" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="U47" s="87"/>
-      <c r="V47" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="W47" s="87"/>
-      <c r="X47" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="Y47" s="87"/>
-      <c r="Z47" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AA47" s="87"/>
-      <c r="AB47" s="104">
-        <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
-        <v>0</v>
-      </c>
-      <c r="AC47" s="87"/>
-      <c r="AD47" s="105"/>
-      <c r="AE47" s="105"/>
-      <c r="AF47" s="87" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A48" s="33">
-        <f t="shared" si="2"/>
-        <v>46</v>
+        <f>A47+1</f>
+        <v>33</v>
       </c>
       <c r="B48" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C48" s="90">
-        <v>2.274</v>
-      </c>
-      <c r="D48" s="63" t="s">
-        <v>109</v>
+        <v>2.7320000000000002</v>
+      </c>
+      <c r="C48" s="88">
+        <f>C47</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D48" s="65" t="s">
+        <v>106</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>107</v>
@@ -7868,20 +7894,20 @@
       <c r="G48" s="43">
         <v>10</v>
       </c>
-      <c r="H48" s="91" t="s">
-        <v>110</v>
+      <c r="H48" s="115" t="s">
+        <v>108</v>
       </c>
       <c r="I48" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="K48" s="14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L48" s="14">
-        <v>0.59</v>
+        <v>7.109</v>
       </c>
       <c r="M48" s="15">
         <v>0.2</v>
@@ -7920,101 +7946,107 @@
         <v>0</v>
       </c>
       <c r="AC48" s="15"/>
-      <c r="AD48" s="92"/>
-      <c r="AE48" s="92"/>
+      <c r="AD48" s="90"/>
+      <c r="AE48" s="90"/>
       <c r="AF48" s="15"/>
     </row>
-    <row r="49" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A49" s="33">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="B49" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C49" s="90">
-        <f>C48+0.001</f>
-        <v>2.2749999999999999</v>
-      </c>
-      <c r="D49" s="63" t="s">
-        <v>109</v>
+        <v>32</v>
+      </c>
+      <c r="B49" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="88">
+        <f>C48-0.001</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="65" t="str">
+        <f>D48</f>
+        <v>8-juil.</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="F49" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G49" s="43">
+        <v>5</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I49" s="13">
         <v>10</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I49" s="14">
-        <v>60</v>
       </c>
       <c r="J49" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K49" s="14">
-        <v>1</v>
-      </c>
-      <c r="L49" s="14">
-        <v>0.54</v>
-      </c>
-      <c r="M49" s="15">
-        <v>3.3329999999999999E-2</v>
-      </c>
-      <c r="N49" s="15"/>
-      <c r="O49" s="55"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="35">
+      <c r="K49" s="13">
+        <v>20</v>
+      </c>
+      <c r="L49" s="13">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="M49" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N49" s="13">
+        <v>30000</v>
+      </c>
+      <c r="O49" s="39">
+        <v>2000</v>
+      </c>
+      <c r="P49" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S49" s="15"/>
-      <c r="T49" s="35">
+      <c r="S49" s="13"/>
+      <c r="T49" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U49" s="15"/>
-      <c r="V49" s="35">
+      <c r="U49" s="13"/>
+      <c r="V49" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W49" s="15"/>
-      <c r="X49" s="35">
+      <c r="W49" s="13"/>
+      <c r="X49" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y49" s="15"/>
-      <c r="Z49" s="35">
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA49" s="15"/>
-      <c r="AB49" s="35">
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC49" s="15"/>
-      <c r="AD49" s="92"/>
-      <c r="AE49" s="92"/>
+      <c r="AD49" s="90"/>
+      <c r="AE49" s="90"/>
       <c r="AF49" s="15"/>
     </row>
-    <row r="50" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A50" s="33">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f>A49+1</f>
+        <v>33</v>
       </c>
       <c r="B50" s="80">
         <v>2.7669999999999999</v>
       </c>
-      <c r="C50" s="90">
-        <f t="shared" ref="C50:C58" si="4">C49+0.001</f>
-        <v>2.2759999999999998</v>
+      <c r="C50" s="88">
+        <f>C49+0.001</f>
+        <v>1E-3</v>
       </c>
       <c r="D50" s="63" t="s">
         <v>109</v>
@@ -8032,16 +8064,16 @@
         <v>111</v>
       </c>
       <c r="I50" s="14">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="J50" s="13" t="s">
         <v>94</v>
       </c>
       <c r="K50" s="14">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="L50" s="14">
-        <v>0.52</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="M50" s="15">
         <v>3.3329999999999999E-2</v>
@@ -8080,101 +8112,107 @@
         <v>0</v>
       </c>
       <c r="AC50" s="15"/>
-      <c r="AD50" s="92"/>
-      <c r="AE50" s="92"/>
+      <c r="AD50" s="90"/>
+      <c r="AE50" s="90"/>
       <c r="AF50" s="15"/>
     </row>
-    <row r="51" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A51" s="33">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="B51" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C51" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2769999999999997</v>
-      </c>
-      <c r="D51" s="63" t="s">
-        <v>109</v>
+        <v>33</v>
+      </c>
+      <c r="B51" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="88">
+        <f>C50-0.001</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="65" t="str">
+        <f>D50</f>
+        <v>11-juil</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="F51" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G51" s="43">
-        <v>10</v>
-      </c>
-      <c r="H51" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I51" s="14">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I51" s="13">
+        <v>6.6666699999999999</v>
       </c>
       <c r="J51" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K51" s="14">
-        <v>3</v>
-      </c>
-      <c r="L51" s="14">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="M51" s="15">
-        <v>3.3329999999999999E-2</v>
-      </c>
-      <c r="N51" s="15"/>
-      <c r="O51" s="55"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="35">
+      <c r="K51" s="13">
+        <v>30</v>
+      </c>
+      <c r="L51" s="13">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="M51" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N51" s="13">
+        <v>30000</v>
+      </c>
+      <c r="O51" s="39">
+        <v>2000</v>
+      </c>
+      <c r="P51" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S51" s="15"/>
-      <c r="T51" s="35">
+      <c r="S51" s="13"/>
+      <c r="T51" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U51" s="15"/>
-      <c r="V51" s="35">
+      <c r="U51" s="13"/>
+      <c r="V51" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W51" s="15"/>
-      <c r="X51" s="35">
+      <c r="W51" s="13"/>
+      <c r="X51" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y51" s="15"/>
-      <c r="Z51" s="35">
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA51" s="15"/>
-      <c r="AB51" s="35">
+      <c r="AA51" s="13"/>
+      <c r="AB51" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC51" s="15"/>
-      <c r="AD51" s="92"/>
-      <c r="AE51" s="92"/>
+      <c r="AD51" s="90"/>
+      <c r="AE51" s="90"/>
       <c r="AF51" s="15"/>
     </row>
-    <row r="52" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A52" s="33">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f>A51+1</f>
+        <v>34</v>
       </c>
       <c r="B52" s="80">
         <v>2.7669999999999999</v>
       </c>
-      <c r="C52" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2779999999999996</v>
+      <c r="C52" s="88">
+        <f>C51+0.002</f>
+        <v>2E-3</v>
       </c>
       <c r="D52" s="63" t="s">
         <v>109</v>
@@ -8192,19 +8230,19 @@
         <v>111</v>
       </c>
       <c r="I52" s="14">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J52" s="13" t="s">
         <v>94</v>
       </c>
       <c r="K52" s="14">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="L52" s="14">
-        <v>0.57899999999999996</v>
+        <v>0.54</v>
       </c>
       <c r="M52" s="15">
-        <v>3.3329999999999999E-2</v>
+        <v>6.6659999999999997E-2</v>
       </c>
       <c r="N52" s="15"/>
       <c r="O52" s="55"/>
@@ -8240,181 +8278,192 @@
         <v>0</v>
       </c>
       <c r="AC52" s="15"/>
-      <c r="AD52" s="92"/>
-      <c r="AE52" s="92"/>
+      <c r="AD52" s="90"/>
+      <c r="AE52" s="90"/>
       <c r="AF52" s="15"/>
     </row>
-    <row r="53" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A53" s="33">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-      <c r="B53" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C53" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2789999999999995</v>
-      </c>
-      <c r="D53" s="63" t="s">
-        <v>109</v>
+        <v>34</v>
+      </c>
+      <c r="B53" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="88">
+        <f>C52-0.001</f>
+        <v>1E-3</v>
+      </c>
+      <c r="D53" s="65" t="str">
+        <f>D52</f>
+        <v>11-juil</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="F53" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G53" s="43">
-        <v>10</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I53" s="14">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I53" s="13">
+        <v>4</v>
       </c>
       <c r="J53" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K53" s="14">
-        <v>5</v>
-      </c>
-      <c r="L53" s="14">
-        <v>0.47599999999999998</v>
-      </c>
-      <c r="M53" s="15">
-        <v>3.3329999999999999E-2</v>
-      </c>
-      <c r="N53" s="15"/>
-      <c r="O53" s="55"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="35">
+      <c r="K53" s="13">
+        <v>50</v>
+      </c>
+      <c r="L53" s="13">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="M53" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N53" s="13">
+        <v>30000</v>
+      </c>
+      <c r="O53" s="39">
+        <v>2000</v>
+      </c>
+      <c r="P53" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S53" s="15"/>
-      <c r="T53" s="35">
+      <c r="S53" s="13"/>
+      <c r="T53" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U53" s="15"/>
-      <c r="V53" s="35">
+      <c r="U53" s="13"/>
+      <c r="V53" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W53" s="15"/>
-      <c r="X53" s="35">
+      <c r="W53" s="13"/>
+      <c r="X53" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y53" s="15"/>
-      <c r="Z53" s="35">
+      <c r="Y53" s="13"/>
+      <c r="Z53" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA53" s="15"/>
-      <c r="AB53" s="35">
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC53" s="15"/>
-      <c r="AD53" s="92"/>
-      <c r="AE53" s="92"/>
+      <c r="AD53" s="90"/>
+      <c r="AE53" s="90"/>
       <c r="AF53" s="15"/>
     </row>
-    <row r="54" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A54" s="33">
-        <f t="shared" si="2"/>
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B54" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C54" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2799999999999994</v>
-      </c>
-      <c r="D54" s="63" t="s">
-        <v>109</v>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C54" s="88">
+        <v>2.72</v>
+      </c>
+      <c r="D54" s="65" t="str">
+        <f>D53</f>
+        <v>11-juil</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G54" s="43">
-        <v>10</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I54" s="14">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" s="13">
+        <v>1</v>
       </c>
       <c r="J54" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K54" s="14">
-        <v>10</v>
-      </c>
-      <c r="L54" s="14">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="M54" s="15">
-        <v>3.3329999999999999E-2</v>
-      </c>
-      <c r="N54" s="15"/>
-      <c r="O54" s="55"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="35">
+      <c r="K54" s="13">
+        <v>20</v>
+      </c>
+      <c r="L54" s="13">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="M54" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="N54" s="13">
+        <v>7000</v>
+      </c>
+      <c r="O54" s="39">
+        <v>1000</v>
+      </c>
+      <c r="P54" s="13">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S54" s="15"/>
-      <c r="T54" s="35">
+      <c r="S54" s="13"/>
+      <c r="T54" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U54" s="15"/>
-      <c r="V54" s="35">
+      <c r="U54" s="13"/>
+      <c r="V54" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W54" s="15"/>
-      <c r="X54" s="35">
+      <c r="W54" s="13"/>
+      <c r="X54" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y54" s="15"/>
-      <c r="Z54" s="35">
+      <c r="Y54" s="13"/>
+      <c r="Z54" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA54" s="15"/>
-      <c r="AB54" s="35">
+      <c r="AA54" s="13"/>
+      <c r="AB54" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC54" s="15"/>
-      <c r="AD54" s="92"/>
-      <c r="AE54" s="92"/>
+      <c r="AD54" s="90"/>
+      <c r="AE54" s="90"/>
       <c r="AF54" s="15"/>
     </row>
-    <row r="55" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A55" s="33">
-        <f t="shared" si="2"/>
-        <v>53</v>
+        <f>A54+1</f>
+        <v>36</v>
       </c>
       <c r="B55" s="80">
         <v>2.7669999999999999</v>
       </c>
-      <c r="C55" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2809999999999993</v>
+      <c r="C55" s="88">
+        <f>C54+0.001</f>
+        <v>2.7210000000000001</v>
       </c>
       <c r="D55" s="63" t="s">
         <v>109</v>
@@ -8432,19 +8481,19 @@
         <v>111</v>
       </c>
       <c r="I55" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J55" s="13" t="s">
         <v>94</v>
       </c>
       <c r="K55" s="14">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="L55" s="14">
-        <v>0.49</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="M55" s="15">
-        <v>3.3329999999999999E-2</v>
+        <v>1.6660000000000001E-2</v>
       </c>
       <c r="N55" s="15"/>
       <c r="O55" s="55"/>
@@ -8480,24 +8529,24 @@
         <v>0</v>
       </c>
       <c r="AC55" s="15"/>
-      <c r="AD55" s="92"/>
-      <c r="AE55" s="92"/>
+      <c r="AD55" s="90"/>
+      <c r="AE55" s="90"/>
       <c r="AF55" s="15"/>
     </row>
-    <row r="56" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A56" s="33">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f>A55+1</f>
+        <v>37</v>
       </c>
       <c r="B56" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C56" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2819999999999991</v>
-      </c>
-      <c r="D56" s="63" t="s">
-        <v>109</v>
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C56" s="88">
+        <f>C55+0.001</f>
+        <v>2.722</v>
+      </c>
+      <c r="D56" s="65" t="s">
+        <v>106</v>
       </c>
       <c r="E56" s="13" t="s">
         <v>107</v>
@@ -8508,23 +8557,23 @@
       <c r="G56" s="43">
         <v>10</v>
       </c>
-      <c r="H56" s="14" t="s">
-        <v>111</v>
+      <c r="H56" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="I56" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="K56" s="14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L56" s="14">
-        <v>0.5</v>
+        <v>7.2229999999999999</v>
       </c>
       <c r="M56" s="15">
-        <v>3.3329999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N56" s="15"/>
       <c r="O56" s="55"/>
@@ -8560,24 +8609,24 @@
         <v>0</v>
       </c>
       <c r="AC56" s="15"/>
-      <c r="AD56" s="92"/>
-      <c r="AE56" s="92"/>
+      <c r="AD56" s="90"/>
+      <c r="AE56" s="90"/>
       <c r="AF56" s="15"/>
     </row>
-    <row r="57" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A57" s="33">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f>A56+1</f>
+        <v>38</v>
       </c>
       <c r="B57" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C57" s="90">
-        <f t="shared" si="4"/>
-        <v>2.282999999999999</v>
-      </c>
-      <c r="D57" s="63" t="s">
-        <v>109</v>
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C57" s="88">
+        <f>C56+0.001</f>
+        <v>2.7229999999999999</v>
+      </c>
+      <c r="D57" s="65" t="s">
+        <v>106</v>
       </c>
       <c r="E57" s="13" t="s">
         <v>107</v>
@@ -8588,23 +8637,23 @@
       <c r="G57" s="43">
         <v>10</v>
       </c>
-      <c r="H57" s="14" t="s">
-        <v>111</v>
+      <c r="H57" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="I57" s="14">
         <v>2</v>
       </c>
       <c r="J57" s="13" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="K57" s="14">
-        <v>30</v>
+        <v>1000</v>
       </c>
       <c r="L57" s="14">
-        <v>0.61799999999999999</v>
+        <v>7.1159999999999997</v>
       </c>
       <c r="M57" s="15">
-        <v>3.3329999999999999E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="N57" s="15"/>
       <c r="O57" s="55"/>
@@ -8640,24 +8689,23 @@
         <v>0</v>
       </c>
       <c r="AC57" s="15"/>
-      <c r="AD57" s="92"/>
-      <c r="AE57" s="92"/>
+      <c r="AD57" s="90"/>
+      <c r="AE57" s="90"/>
       <c r="AF57" s="15"/>
     </row>
-    <row r="58" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A58" s="33">
-        <f t="shared" si="2"/>
-        <v>56</v>
+        <f>A57+1</f>
+        <v>39</v>
       </c>
       <c r="B58" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C58" s="90">
-        <f t="shared" si="4"/>
-        <v>2.2839999999999989</v>
-      </c>
-      <c r="D58" s="63" t="s">
-        <v>109</v>
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C58" s="88">
+        <v>2.7120000000000002</v>
+      </c>
+      <c r="D58" s="65" t="s">
+        <v>106</v>
       </c>
       <c r="E58" s="13" t="s">
         <v>107</v>
@@ -8668,76 +8716,76 @@
       <c r="G58" s="43">
         <v>10</v>
       </c>
-      <c r="H58" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I58" s="14">
+      <c r="H58" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I58" s="13">
         <v>1</v>
       </c>
       <c r="J58" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="K58" s="14">
-        <v>60</v>
-      </c>
-      <c r="L58" s="14">
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="M58" s="15">
-        <v>3.3329999999999999E-2</v>
-      </c>
-      <c r="N58" s="15"/>
-      <c r="O58" s="55"/>
-      <c r="P58" s="14"/>
-      <c r="Q58" s="15"/>
-      <c r="R58" s="35">
+        <v>34</v>
+      </c>
+      <c r="K58" s="13">
+        <v>20</v>
+      </c>
+      <c r="L58" s="13">
+        <v>7.27</v>
+      </c>
+      <c r="M58" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="N58" s="13"/>
+      <c r="O58" s="39"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S58" s="15"/>
-      <c r="T58" s="35">
+      <c r="S58" s="13"/>
+      <c r="T58" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U58" s="15"/>
-      <c r="V58" s="35">
+      <c r="U58" s="13"/>
+      <c r="V58" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W58" s="15"/>
-      <c r="X58" s="35">
+      <c r="W58" s="13"/>
+      <c r="X58" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y58" s="15"/>
-      <c r="Z58" s="35">
+      <c r="Y58" s="13"/>
+      <c r="Z58" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA58" s="15"/>
-      <c r="AB58" s="35">
+      <c r="AA58" s="13"/>
+      <c r="AB58" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC58" s="15"/>
-      <c r="AD58" s="92"/>
-      <c r="AE58" s="92"/>
+      <c r="AD58" s="90"/>
+      <c r="AE58" s="90"/>
       <c r="AF58" s="15"/>
     </row>
-    <row r="59" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A59" s="33">
-        <f t="shared" si="2"/>
-        <v>57</v>
+        <f>A58+1</f>
+        <v>40</v>
       </c>
       <c r="B59" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C59" s="90">
-        <f>C58+0.002</f>
-        <v>2.2859999999999987</v>
-      </c>
-      <c r="D59" s="63" t="s">
-        <v>109</v>
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C59" s="88">
+        <f>C58+0.001</f>
+        <v>2.7130000000000001</v>
+      </c>
+      <c r="D59" s="65" t="s">
+        <v>106</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>107</v>
@@ -8748,76 +8796,76 @@
       <c r="G59" s="43">
         <v>10</v>
       </c>
-      <c r="H59" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I59" s="14">
-        <v>2</v>
+      <c r="H59" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I59" s="13">
+        <v>1</v>
       </c>
       <c r="J59" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="K59" s="14">
-        <v>30</v>
-      </c>
-      <c r="L59" s="14">
-        <v>0.54</v>
-      </c>
-      <c r="M59" s="15">
-        <v>6.6659999999999997E-2</v>
-      </c>
-      <c r="N59" s="15"/>
-      <c r="O59" s="55"/>
-      <c r="P59" s="14"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="35">
+        <v>34</v>
+      </c>
+      <c r="K59" s="13">
+        <v>20</v>
+      </c>
+      <c r="L59" s="13">
+        <v>7.0350000000000001</v>
+      </c>
+      <c r="M59" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="N59" s="13"/>
+      <c r="O59" s="39"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Min Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="S59" s="15"/>
-      <c r="T59" s="35">
+      <c r="S59" s="13"/>
+      <c r="T59" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Dot         pC]]*Table2[[#This Row],[Max Dot DF]]</f>
         <v>0</v>
       </c>
-      <c r="U59" s="15"/>
-      <c r="V59" s="35">
+      <c r="U59" s="13"/>
+      <c r="V59" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="W59" s="15"/>
-      <c r="X59" s="35">
+      <c r="W59" s="13"/>
+      <c r="X59" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Line μC/cm]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Line DF]]</f>
         <v>0</v>
       </c>
-      <c r="Y59" s="15"/>
-      <c r="Z59" s="35">
+      <c r="Y59" s="13"/>
+      <c r="Z59" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Min Area DF]]</f>
         <v>0</v>
       </c>
-      <c r="AA59" s="15"/>
-      <c r="AB59" s="35">
+      <c r="AA59" s="13"/>
+      <c r="AB59" s="13">
         <f>Table2[[#This Row],[Design dose factor]]*Table2[[#This Row],[Loop factor]]*Table2[[#This Row],[Area μC/cm^2]]*Table2[[#This Row],[Area/Line step size (𝝁m)]]*Table2[[#This Row],[Max Area DF]]</f>
         <v>0</v>
       </c>
       <c r="AC59" s="15"/>
-      <c r="AD59" s="92"/>
-      <c r="AE59" s="92"/>
+      <c r="AD59" s="90"/>
+      <c r="AE59" s="90"/>
       <c r="AF59" s="15"/>
     </row>
-    <row r="60" spans="1:32" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:32" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A60" s="33">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f>A59+1</f>
+        <v>41</v>
       </c>
       <c r="B60" s="80">
-        <v>2.7669999999999999</v>
-      </c>
-      <c r="C60" s="90">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="C60" s="88">
         <f>C59+0.001</f>
-        <v>2.2869999999999986</v>
-      </c>
-      <c r="D60" s="63" t="s">
-        <v>109</v>
+        <v>2.714</v>
+      </c>
+      <c r="D60" s="65" t="s">
+        <v>106</v>
       </c>
       <c r="E60" s="13" t="s">
         <v>107</v>
@@ -8828,23 +8876,23 @@
       <c r="G60" s="43">
         <v>10</v>
       </c>
-      <c r="H60" s="14" t="s">
-        <v>111</v>
+      <c r="H60" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="I60" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J60" s="13" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="K60" s="14">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L60" s="14">
-        <v>0.57199999999999995</v>
+        <v>7.2149999999999999</v>
       </c>
       <c r="M60" s="15">
-        <v>1.6660000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N60" s="15"/>
       <c r="O60" s="55"/>
@@ -8880,8 +8928,8 @@
         <v>0</v>
       </c>
       <c r="AC60" s="15"/>
-      <c r="AD60" s="92"/>
-      <c r="AE60" s="92"/>
+      <c r="AD60" s="90"/>
+      <c r="AE60" s="90"/>
       <c r="AF60" s="15"/>
     </row>
   </sheetData>
@@ -8928,19 +8976,19 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="12"/>
-    <col min="3" max="3" width="16.83203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="6.796875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="12"/>
+    <col min="3" max="3" width="16.796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="19.69921875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16.296875" style="12" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="12"/>
+    <col min="7" max="7" width="13.69921875" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -8982,7 +9030,7 @@
       </c>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>40</v>
       </c>
@@ -9005,7 +9053,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -9030,7 +9078,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="78" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>55</v>
@@ -9053,7 +9101,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
@@ -9078,7 +9126,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>59</v>
       </c>
@@ -9103,7 +9151,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -9118,7 +9166,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -9133,7 +9181,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -9148,7 +9196,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -9163,7 +9211,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -9178,7 +9226,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -9193,7 +9241,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -9208,7 +9256,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -9223,7 +9271,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="3"/>
@@ -9252,7 +9300,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>